<commit_message>
Updated for 3rd april
</commit_message>
<xml_diff>
--- a/Daily Status update Report 03042020.xlsx
+++ b/Daily Status update Report 03042020.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="10"/>
@@ -19,7 +19,7 @@
     <sheet name="01-Apr" sheetId="11" r:id="rId10"/>
     <sheet name="03-Apr" sheetId="12" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="119">
   <si>
     <t>Employee Name</t>
   </si>
@@ -380,13 +380,19 @@
   </si>
   <si>
     <t>Understanding the SLA document; Planned discussion on the Settlement module</t>
+  </si>
+  <si>
+    <t>Understanding Modified trade flow For following scenarios 1.Trade Insert - for Cash Market  2. Rectify Quantity</t>
+  </si>
+  <si>
+    <t>Discussion on SLA document for PT; Cucumber set up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -822,21 +828,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -847,7 +853,7 @@
     <col min="7" max="7" width="117.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -870,7 +876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -893,7 +899,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -916,7 +922,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -939,7 +945,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -962,7 +968,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -985,7 +991,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1008,7 +1014,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1121,7 +1127,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1149,14 +1155,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD14"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1167,7 +1173,7 @@
     <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1190,7 +1196,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1236,7 +1242,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1282,7 +1288,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1305,7 +1311,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1328,7 +1334,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1351,7 +1357,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -1420,7 +1426,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -1443,7 +1449,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -1466,7 +1472,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -1496,14 +1502,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1514,7 +1520,7 @@
     <col min="7" max="7" width="166" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1537,7 +1543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1558,7 +1564,7 @@
       </c>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1579,7 +1585,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1600,7 +1606,7 @@
       </c>
       <c r="G4" s="31"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1621,7 +1627,7 @@
       </c>
       <c r="G5" s="31"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1642,7 +1648,7 @@
       </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1663,7 +1669,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1684,7 +1690,7 @@
       </c>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1705,7 +1711,7 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -1728,7 +1734,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -1747,9 +1753,11 @@
       <c r="F11" s="34">
         <v>0.75</v>
       </c>
-      <c r="G11" s="32"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -1768,9 +1776,11 @@
       <c r="F12" s="34">
         <v>0.75</v>
       </c>
-      <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -1791,7 +1801,7 @@
       </c>
       <c r="G13" s="32"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -1814,18 +1824,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1836,7 +1847,7 @@
     <col min="7" max="7" width="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1859,7 +1870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1882,7 +1893,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1905,7 +1916,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1928,7 +1939,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1951,7 +1962,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1974,7 +1985,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1997,7 +2008,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2020,7 +2031,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2043,7 +2054,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2066,7 +2077,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2089,7 +2100,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2112,7 +2123,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2142,14 +2153,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2160,7 +2171,7 @@
     <col min="7" max="7" width="136.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2183,7 +2194,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2206,7 +2217,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2229,7 +2240,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2252,7 +2263,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2275,7 +2286,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2298,7 +2309,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2321,7 +2332,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2344,7 +2355,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2367,7 +2378,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2390,7 +2401,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2413,7 +2424,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2436,7 +2447,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2466,14 +2477,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2484,7 +2495,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2507,7 +2518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2530,7 +2541,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2553,7 +2564,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2576,7 +2587,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2599,7 +2610,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2622,7 +2633,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2645,7 +2656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2668,7 +2679,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2691,7 +2702,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2714,7 +2725,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2737,7 +2748,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2760,7 +2771,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2783,7 +2794,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2813,14 +2824,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -2831,7 +2842,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2854,7 +2865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2877,7 +2888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2900,7 +2911,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2923,7 +2934,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2946,7 +2957,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2969,7 +2980,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2992,7 +3003,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3015,7 +3026,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3038,7 +3049,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3061,7 +3072,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3084,7 +3095,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3107,7 +3118,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3130,7 +3141,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3160,14 +3171,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3178,7 +3189,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3201,7 +3212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3224,7 +3235,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3247,7 +3258,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3270,7 +3281,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3293,7 +3304,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3316,7 +3327,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3339,7 +3350,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3362,7 +3373,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3385,7 +3396,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3408,7 +3419,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3431,7 +3442,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3454,7 +3465,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3477,7 +3488,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3507,14 +3518,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3525,7 +3536,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3548,7 +3559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3571,7 +3582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3594,7 +3605,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3617,7 +3628,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3640,7 +3651,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3663,7 +3674,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3686,7 +3697,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3709,7 +3720,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3732,7 +3743,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3755,7 +3766,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3778,7 +3789,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3801,7 +3812,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3824,7 +3835,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3854,14 +3865,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -3872,7 +3883,7 @@
     <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
@@ -3895,7 +3906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -3918,7 +3929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -3941,7 +3952,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -3964,7 +3975,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -3987,7 +3998,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -4010,7 +4021,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -4033,7 +4044,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -4056,7 +4067,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -4079,7 +4090,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -4102,7 +4113,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -4125,7 +4136,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -4148,7 +4159,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -4171,7 +4182,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -4201,14 +4212,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -4219,7 +4230,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4242,7 +4253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4265,7 +4276,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4288,7 +4299,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4311,7 +4322,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4334,7 +4345,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4357,7 +4368,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4380,7 +4391,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4403,7 +4414,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4426,7 +4437,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -4449,7 +4460,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -4472,7 +4483,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -4495,7 +4506,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -4518,7 +4529,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="33">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
updated gautami's status for 3rd april
</commit_message>
<xml_diff>
--- a/Daily Status update Report 03042020.xlsx
+++ b/Daily Status update Report 03042020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="120">
   <si>
     <t>Employee Name</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>Discussion on SLA document for PT; Cucumber set up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Git Basic Understanding Complete ; </t>
   </si>
 </sst>
 </file>
@@ -829,7 +832,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1506,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1800,7 +1803,9 @@
       <c r="F13" s="34">
         <v>0.75</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="32" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="33">
@@ -1833,7 +1838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated status for 7th April- me and gautami
</commit_message>
<xml_diff>
--- a/Daily Status update Report 03042020.xlsx
+++ b/Daily Status update Report 03042020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="122">
   <si>
     <t>Employee Name</t>
   </si>
@@ -390,6 +390,12 @@
   </si>
   <si>
     <t xml:space="preserve">Git Basic Understanding Complete ; </t>
+  </si>
+  <si>
+    <t>Working on keyword driven framework</t>
+  </si>
+  <si>
+    <t>Understanding SLA document and Interface service flow; working on cucumber</t>
   </si>
 </sst>
 </file>
@@ -832,7 +838,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1509,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1838,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2105,7 +2111,9 @@
       <c r="F12" s="34">
         <v>0.75</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="32" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="32">
@@ -2126,7 +2134,9 @@
       <c r="F13" s="34">
         <v>0.75</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="32" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="33">

</xml_diff>